<commit_message>
Updated Test Cases and Created Blank
Updated and ran test cases for misc scenarios.

Also created a blank (untested) version of the test cases in case some unholy force compelled us to re-test in future milestones
</commit_message>
<xml_diff>
--- a/Documentation/TestCases.xlsx
+++ b/Documentation/TestCases.xlsx
@@ -8,19 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\School\CST-341\OtherFileNonsense\Workspace\SpringCLC\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11382B2-BF68-4E7A-B063-85F1079C719E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B953AC0D-8749-427D-922F-30D431C8F9CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="7" xr2:uid="{59774C4E-BB0C-46C8-9D53-717A2C046DC2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="3" activeTab="11" xr2:uid="{59774C4E-BB0C-46C8-9D53-717A2C046DC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Use" sheetId="1" r:id="rId1"/>
     <sheet name="Login Validation" sheetId="5" r:id="rId2"/>
-    <sheet name="Registration Use" sheetId="2" r:id="rId3"/>
-    <sheet name="Registration Validation" sheetId="6" r:id="rId4"/>
-    <sheet name="Album Use" sheetId="3" r:id="rId5"/>
-    <sheet name="Album Validation" sheetId="7" r:id="rId6"/>
-    <sheet name="Song Use" sheetId="4" r:id="rId7"/>
-    <sheet name="Song Validation" sheetId="8" r:id="rId8"/>
+    <sheet name="Login (Misc)" sheetId="9" r:id="rId3"/>
+    <sheet name="Registration Use" sheetId="2" r:id="rId4"/>
+    <sheet name="Registration Validation" sheetId="6" r:id="rId5"/>
+    <sheet name="Registration (Misc)" sheetId="10" r:id="rId6"/>
+    <sheet name="Album Use" sheetId="3" r:id="rId7"/>
+    <sheet name="Album Validation" sheetId="7" r:id="rId8"/>
+    <sheet name="Album (Misc)" sheetId="11" r:id="rId9"/>
+    <sheet name="Song Use" sheetId="4" r:id="rId10"/>
+    <sheet name="Song Validation" sheetId="8" r:id="rId11"/>
+    <sheet name="Song (Misc)" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="187">
   <si>
     <t>Project Name:</t>
   </si>
@@ -480,12 +484,218 @@
 2. Fill out both fields with 45 characters 
 3. Press the "edit song" button</t>
   </si>
+  <si>
+    <t>Low-High (Depending on test)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(High Priority) Incorrect Login Credentials </t>
+  </si>
+  <si>
+    <t>If a user submits incorrect login credentials, an error message is returned</t>
+  </si>
+  <si>
+    <t>Log in with an username and password that fit form validation</t>
+  </si>
+  <si>
+    <t>Username: Hello
+Password: WorldWorld</t>
+  </si>
+  <si>
+    <t>Error message warns of incorrect credentials</t>
+  </si>
+  <si>
+    <t>(High Priority) Database Disconnect is Handled</t>
+  </si>
+  <si>
+    <t>This module handles a database connection failure appropriately</t>
+  </si>
+  <si>
+    <t>Turn off MAMP or sabatoge database connection and attempt to use module normally</t>
+  </si>
+  <si>
+    <t>Error message states that an unexpected error has occurred</t>
+  </si>
+  <si>
+    <t>(Low Priority) A logged on user cannot log in again</t>
+  </si>
+  <si>
+    <t>Forcibly navigating back to the login page while logged in returns some manner of error</t>
+  </si>
+  <si>
+    <t>1. Log in with valid credentials
+2. Navigate directly to localhost:8080/SpringCLC/login/portal
+3. Attempt to log in</t>
+  </si>
+  <si>
+    <t>Username: MSillanp
+Password: password</t>
+  </si>
+  <si>
+    <t>App allows second log in</t>
+  </si>
+  <si>
+    <t>Pass?</t>
+  </si>
+  <si>
+    <t>Not sure this one matters, at the end of the day</t>
+  </si>
+  <si>
+    <t>(Low Priority) A logged on user cannot log in as a different user</t>
+  </si>
+  <si>
+    <t>Forcibly navigating back to the login page and logging in as a different user while logged in returns some manner of error</t>
+  </si>
+  <si>
+    <t>1. Log in with valid credentials
+2. Navigate directly to localhost:8080/SpringCLC/login/portal
+3. Attempt to log in as a different user</t>
+  </si>
+  <si>
+    <t>Username: MSillanp
+Password: password
+Username: RedWolfHood
+Password: password</t>
+  </si>
+  <si>
+    <t>App logs in as second user, seems to overwrite first user</t>
+  </si>
+  <si>
+    <t>This is a weird thing for a user to try and do. At some point we could put measures against it but it doesn’t really hurt anyone</t>
+  </si>
+  <si>
+    <t>(High Priority) A user cannot register with a duplicate username</t>
+  </si>
+  <si>
+    <t>This module does not allow a user to register with a username that is already taken</t>
+  </si>
+  <si>
+    <t>1. A user fills out the form with valid data, except for a username which is already taken
+2. User attempts to submit the form</t>
+  </si>
+  <si>
+    <t>Username: Msillanp</t>
+  </si>
+  <si>
+    <t>Error Message states that that username is not available</t>
+  </si>
+  <si>
+    <t>Error Message states that "email" is not available</t>
+  </si>
+  <si>
+    <t>Close Enough</t>
+  </si>
+  <si>
+    <t>We need to change the word email to username in the return message at some point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Medium Priority) Duplicate Album Creation </t>
+  </si>
+  <si>
+    <t>An album cannot be created if that album already exists</t>
+  </si>
+  <si>
+    <t>1. Press the "Add Album" button to open the modal
+2. Fill out the form with duplicate Name and artist fields (For this user)
+3.Click "Create Album"</t>
+  </si>
+  <si>
+    <t>Name: NewAlbum
+Artist: NewArtist</t>
+  </si>
+  <si>
+    <t>Error message states that this album already exists</t>
+  </si>
+  <si>
+    <t>Database is not affected</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>Error message states that this album already exists
+HOWEVER, this happens even if a different user attempts to add the same album</t>
+  </si>
+  <si>
+    <t>The current logic doesn't work the way we have the app set up. If the created albums went somewhere that all users could browse, it would work, but as it is, each user should be allowed to create the same album</t>
+  </si>
+  <si>
+    <t>(Low Priority) Attempting to act on a deleted album</t>
+  </si>
+  <si>
+    <t>If a user opens an album, opens a new tab and deletes that album, then attempts to act on the album in the first tab, the program should handle it</t>
+  </si>
+  <si>
+    <t>1. Access a certain album
+2. In a new tab, open then delete that album
+3. Attempt to edit, add to, or delete that album</t>
+  </si>
+  <si>
+    <t>Database is not affected by second action</t>
+  </si>
+  <si>
+    <t>Error message states "There was a problem with [updating] your album". This means the operation is passing the logical checks and not throwing  any exceptions- including SQL- but is failing as an action with no result</t>
+  </si>
+  <si>
+    <t>debatable</t>
+  </si>
+  <si>
+    <r>
+      <t>On one hand, the application is handling the issue. 
+On the other, it seems to be bypassing logic that should throw an exception.
+On the other hand, this is an obscure error that a user Shouldn't</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>™ encounter
+On the final hand, it could mean that our code warrants investigation</t>
+    </r>
+  </si>
+  <si>
+    <t>(Low Priority) Attempting to act on a deleted song</t>
+  </si>
+  <si>
+    <t>If a user opens an album, opens a new tab and deletes a song, then attempts to act on the song in the first tab, the program should handle it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Medium Priority) Duplicate Song Creation </t>
+  </si>
+  <si>
+    <t>A song cannot be created if that song already exists</t>
+  </si>
+  <si>
+    <t>Name: NewSong
+Artist: NewArtist</t>
+  </si>
+  <si>
+    <t>Error message states that this song already exists in this album</t>
+  </si>
+  <si>
+    <t>1. Access a certain album
+2. In a new tab, open then delete a song in that album
+3. Attempt to edit or delete that song in the first tab</t>
+  </si>
+  <si>
+    <t>Error message states that this song already exists, but only within the same album</t>
+  </si>
+  <si>
+    <t>1. Press the "Add song" button to open the modal
+2. Fill out the form with duplicate Name and artist fields (For this album)
+3.Click "Create song"</t>
+  </si>
+  <si>
+    <t>Error message states "There was a problem with [updating] your song". This means the operation is passing the logical checks and not throwing  any exceptions- including SQL- but is failing as an action with no result</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,6 +759,12 @@
     <font>
       <sz val="8"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -694,7 +910,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -773,6 +989,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1122,7 +1341,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1144,7 +1363,7 @@
       <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1168,12 +1387,12 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="31">
         <v>5</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
@@ -1195,28 +1414,28 @@
       <c r="A6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="29"/>
     </row>
     <row r="7" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="29"/>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
@@ -1298,6 +1517,847 @@
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="B7:C7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECAE631C-5204-4326-B681-9A75BB27D9DE}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10">
+        <v>43779</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="30"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="12">
+        <v>43779</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="31">
+        <v>5</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="3"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>1</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>2</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
+        <v>3</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C298088C-5687-4AA9-BAF1-49548B226F74}">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="23" style="13" customWidth="1"/>
+    <col min="3" max="3" width="48.77734375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.109375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="52.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10">
+        <v>43779</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="30"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="12">
+        <v>43779</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="31">
+        <v>5</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="3"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="13">
+        <v>2</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="13">
+        <v>3</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="13">
+        <v>2</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B27E67-9BC1-441B-B114-441632180206}">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="50.77734375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="56.88671875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="44.44140625" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10">
+        <v>43779</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="30"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="12">
+        <v>43779</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="31">
+        <v>5</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="3"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>1</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>2</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" ht="163.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
+        <v>3</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1327,7 +2387,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1349,7 +2409,7 @@
       <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1373,12 +2433,12 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="31">
         <v>5</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
@@ -1400,28 +2460,28 @@
       <c r="A6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="29"/>
     </row>
     <row r="7" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="29"/>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
@@ -1538,6 +2598,305 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B1330E-88AC-46AA-81E4-71525AE7C87D}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.21875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.77734375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.21875" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.21875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10">
+        <v>43779</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="30"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="12">
+        <v>43779</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="31">
+        <v>5</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="3"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="29"/>
+    </row>
+    <row r="7" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="29"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="29"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>1</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>2</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
+        <v>3</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="13">
+        <v>3</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8360C6E5-DBEE-48B2-952E-1CC4A4A00D48}">
   <dimension ref="A1:J11"/>
   <sheetViews>
@@ -1561,7 +2920,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1583,7 +2942,7 @@
       <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1607,12 +2966,12 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="31">
         <v>5</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
@@ -1736,7 +3095,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C345FFF2-CE33-4A69-ACA9-DE449C5E6DBD}">
   <dimension ref="A1:J13"/>
   <sheetViews>
@@ -1760,7 +3119,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1782,7 +3141,7 @@
       <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1806,12 +3165,12 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="31">
         <v>5</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
@@ -1993,12 +3352,248 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165093C1-BACC-45BA-B8E1-B42F17B9284D}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="39.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.77734375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="35.109375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="40.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10">
+        <v>43779</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="30"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="12">
+        <v>43779</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="31">
+        <v>5</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="3"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>1</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1957E8-C9CC-4BCE-A884-8F988729911F}">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2017,7 +3612,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2039,7 +3634,7 @@
       <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2063,12 +3658,12 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="31">
         <v>5</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
@@ -2280,12 +3875,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32DDBC50-3963-4165-AB91-1E1ECEA69C1D}">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2304,7 +3899,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2326,7 +3921,7 @@
       <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2350,12 +3945,12 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="31">
         <v>5</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
@@ -2567,37 +4162,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECAE631C-5204-4326-B681-9A75BB27D9DE}">
-  <dimension ref="A1:J13"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9C71AF-CFC4-4147-93EE-0D5D316F3791}">
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="A12" sqref="A12:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.109375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.6640625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="54.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="13" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="45.21875" style="13" customWidth="1"/>
+    <col min="7" max="7" width="35.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.6640625" style="13" customWidth="1"/>
     <col min="9" max="9" width="9.109375" style="13" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="51.33203125" style="13" customWidth="1"/>
     <col min="11" max="16384" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="27" t="s">
         <v>20</v>
       </c>
       <c r="D1" s="15" t="s">
@@ -2613,12 +4208,12 @@
       <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>23</v>
+      <c r="C2" s="27" t="s">
+        <v>22</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>4</v>
@@ -2637,12 +4232,12 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="31">
         <v>5</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
@@ -2664,29 +4259,24 @@
       <c r="A6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="11" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="25"/>
+      <c r="B7" s="11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>8</v>
+      <c r="B8" s="11" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2701,7 +4291,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
@@ -2733,92 +4323,102 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>1</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>67</v>
+        <v>136</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>71</v>
+        <v>25</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>71</v>
+        <v>25</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>2</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>73</v>
+        <v>161</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>74</v>
+        <v>162</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>75</v>
+        <v>163</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>77</v>
+        <v>164</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>165</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>78</v>
+        <v>166</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>77</v>
+        <v>168</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>3</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>80</v>
+        <v>170</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>81</v>
+        <v>172</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>84</v>
+        <v>25</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>84</v>
+        <v>173</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>38</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2826,306 +4426,6 @@
     <mergeCell ref="C3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C298088C-5687-4AA9-BAF1-49548B226F74}">
-  <dimension ref="A1:J16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.109375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="23" style="13" customWidth="1"/>
-    <col min="3" max="3" width="48.77734375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.109375" style="13" customWidth="1"/>
-    <col min="8" max="8" width="52.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="13" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" style="13" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="13"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="10">
-        <v>43779</v>
-      </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="12">
-        <v>43779</v>
-      </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="30">
-        <v>5</v>
-      </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C5" s="3"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-    </row>
-    <row r="6" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-    </row>
-    <row r="7" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="25"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="11"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
-        <v>1</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="13">
-        <v>2</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="13">
-        <v>3</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="13">
-        <v>2</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C3:F3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>